<commit_message>
i think its clean
</commit_message>
<xml_diff>
--- a/merge/test/merged_blob/metrics_unified.xlsx
+++ b/merge/test/merged_blob/metrics_unified.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Run</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">test_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_panic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_thr_corrected</t>
   </si>
   <si>
     <t xml:space="preserve">test_2</t>
@@ -105,7 +111,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +122,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF6F9D4"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -174,6 +186,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,7 +246,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -254,10 +270,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -351,52 +367,52 @@
         <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.923951657613118</v>
+        <v>0.91621883392334</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.868123333565546</v>
+        <v>0.882291136213956</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.92177998031033</v>
+        <v>0.876495965690433</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0.0748869272008949</v>
+        <v>0.0625373365549312</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.894147413569714</v>
+        <v>0.879384003463087</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.928272752754526</v>
+        <v>0.91144865904875</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0.924038874308268</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0.869336364404107</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>0.920330879581153</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0.0739780864160065</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0.894107106885734</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0.927802294900471</v>
+      <c r="D5" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0.923691520690918</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>0.867315457272158</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0.922066260723838</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>0.0754392886588325</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>0.893853237139996</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>0.928579205321654</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,22 +424,22 @@
         <v>28</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0.923273315429688</v>
+        <v>0.923951657613118</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.86823204737871</v>
+        <v>0.868123333565546</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.919328186538201</v>
+        <v>0.92177998031033</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>0.0746168257071361</v>
+        <v>0.0748869272008949</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.893049843542357</v>
+        <v>0.894147413569714</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.926879260472358</v>
+        <v>0.928272752754526</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,22 +451,22 @@
         <v>28</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0.923355700174968</v>
+        <v>0.924038874308268</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.869396111426876</v>
+        <v>0.869336364404107</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.91793805701976</v>
+        <v>0.920330879581153</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.0737469388660007</v>
+        <v>0.0739780864160065</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.893007912445723</v>
+        <v>0.894107106885734</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.926504241213289</v>
+        <v>0.927802294900471</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,21 +478,73 @@
         <v>28</v>
       </c>
       <c r="E8" s="0" t="n">
+        <v>0.923273315429688</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.86823204737871</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.919328186538201</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.0746168257071361</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.893049843542357</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.926879260472358</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.923355700174968</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.869396111426876</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.91793805701976</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.0737469388660007</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.893007912445723</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0.926504241213289</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>0.923165346781413</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F10" s="0" t="n">
         <v>0.87699065830607</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>0.906667658764841</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>0.0680116732244994</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>0.891582271464148</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>0.923365849107335</v>
       </c>
     </row>

</xml_diff>